<commit_message>
Upgrade minor fix to KenpoFlashcardsProject-v4.5.2 v28 Sync Description
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CCC7F5-9CC8-455A-A4BB-042864A58A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC8F93-F7DB-4C66-9D0A-519AB39B7769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24300" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24300" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List with Pending or Done" sheetId="1" r:id="rId1"/>
@@ -1937,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D388"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -3561,18 +3561,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="70" style="1" customWidth="1"/>
-    <col min="2" max="3" width="28" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="60" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="57" customHeight="1">
+    <row r="1" spans="1:6" ht="23.25" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -3608,7 +3611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="120">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="120">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -3644,7 +3647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+    <row r="5" spans="1:6" ht="105">
       <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="120">
       <c r="A6" s="14" t="s">
         <v>58</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+    <row r="7" spans="1:6" ht="225">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
@@ -3698,7 +3701,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
@@ -3714,7 +3717,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+    <row r="9" spans="1:6" ht="75">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="270">
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
@@ -3750,7 +3753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="135">
       <c r="A11" s="14" t="s">
         <v>66</v>
       </c>
@@ -3768,7 +3771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="14" t="s">
         <v>68</v>
       </c>
@@ -3784,7 +3787,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+    <row r="13" spans="1:6" ht="120">
       <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
@@ -3800,7 +3803,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="14" t="s">
         <v>69</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="90">
       <c r="A15" s="14" t="s">
         <v>19</v>
       </c>
@@ -3834,7 +3837,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="14" t="s">
         <v>20</v>
       </c>
@@ -3850,7 +3853,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="240">
       <c r="A17" s="14" t="s">
         <v>21</v>
       </c>
@@ -3868,7 +3871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="300">
       <c r="A18" s="14" t="s">
         <v>73</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+    <row r="19" spans="1:6" ht="45">
       <c r="A19" s="14" t="s">
         <v>74</v>
       </c>
@@ -3902,7 +3905,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="120">
       <c r="A20" s="14" t="s">
         <v>75</v>
       </c>
@@ -3918,7 +3921,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="45">
       <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
@@ -3934,7 +3937,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
+    <row r="22" spans="1:6" ht="45">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
@@ -3950,7 +3953,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1">
+    <row r="23" spans="1:6" ht="90">
       <c r="A23" s="14" t="s">
         <v>76</v>
       </c>
@@ -3968,7 +3971,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+    <row r="24" spans="1:6" ht="165">
       <c r="A24" s="14" t="s">
         <v>78</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1">
+    <row r="25" spans="1:6" ht="150">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -4004,7 +4007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1">
+    <row r="26" spans="1:6" ht="90">
       <c r="A26" s="14" t="s">
         <v>30</v>
       </c>
@@ -4022,7 +4025,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1">
+    <row r="27" spans="1:6" ht="45">
       <c r="A27" s="14" t="s">
         <v>83</v>
       </c>
@@ -4038,7 +4041,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="90">
       <c r="A28" s="14" t="s">
         <v>32</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
+    <row r="29" spans="1:6" ht="45">
       <c r="A29" s="14" t="s">
         <v>33</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1">
+    <row r="30" spans="1:6" ht="90">
       <c r="A30" s="14" t="s">
         <v>85</v>
       </c>
@@ -4090,7 +4093,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1">
+    <row r="31" spans="1:6" ht="105">
       <c r="A31" s="14" t="s">
         <v>35</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
+    <row r="32" spans="1:6" ht="90">
       <c r="A32" s="14" t="s">
         <v>88</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1">
+    <row r="33" spans="1:6" ht="90">
       <c r="A33" s="14" t="s">
         <v>37</v>
       </c>
@@ -4144,7 +4147,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1">
+    <row r="34" spans="1:6" ht="105">
       <c r="A34" s="14" t="s">
         <v>38</v>
       </c>
@@ -4160,7 +4163,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1">
+    <row r="35" spans="1:6" ht="105">
       <c r="A35" s="14" t="s">
         <v>39</v>
       </c>
@@ -4176,7 +4179,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1">
+    <row r="36" spans="1:6" ht="60">
       <c r="A36" s="14" t="s">
         <v>40</v>
       </c>
@@ -4192,7 +4195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1">
+    <row r="37" spans="1:6" ht="45">
       <c r="A37" s="14" t="s">
         <v>41</v>
       </c>
@@ -4208,7 +4211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1">
+    <row r="38" spans="1:6" ht="45">
       <c r="A38" s="14" t="s">
         <v>42</v>
       </c>
@@ -4224,7 +4227,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1">
+    <row r="39" spans="1:6" ht="45">
       <c r="A39" s="14" t="s">
         <v>43</v>
       </c>
@@ -4240,7 +4243,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1">
+    <row r="40" spans="1:6" ht="45">
       <c r="A40" s="14" t="s">
         <v>92</v>
       </c>
@@ -4256,7 +4259,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1">
+    <row r="41" spans="1:6" ht="45">
       <c r="A41" s="14" t="s">
         <v>45</v>
       </c>
@@ -4272,7 +4275,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1">
+    <row r="42" spans="1:6" ht="45">
       <c r="A42" s="14" t="s">
         <v>46</v>
       </c>
@@ -4496,6 +4499,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4503,18 +4507,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A2:XFD42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="70" style="1" customWidth="1"/>
-    <col min="2" max="3" width="28" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="60" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.5" customHeight="1">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -4550,7 +4557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1">
+    <row r="3" spans="1:6" ht="90">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -4568,7 +4575,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1">
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -4584,7 +4591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1">
+    <row r="5" spans="1:6" ht="90">
       <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
@@ -4602,7 +4609,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1">
+    <row r="6" spans="1:6" ht="105">
       <c r="A6" s="14" t="s">
         <v>58</v>
       </c>
@@ -4618,7 +4625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.5" customHeight="1">
+    <row r="7" spans="1:6" ht="180">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
@@ -4636,7 +4643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.5" customHeight="1">
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
@@ -4652,7 +4659,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.5" customHeight="1">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
@@ -4668,7 +4675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.5" customHeight="1">
+    <row r="10" spans="1:6" ht="225">
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
@@ -4686,7 +4693,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.5" customHeight="1">
+    <row r="11" spans="1:6" ht="120">
       <c r="A11" s="14" t="s">
         <v>66</v>
       </c>
@@ -4704,7 +4711,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.5" customHeight="1">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="14" t="s">
         <v>68</v>
       </c>
@@ -4720,7 +4727,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19.5" customHeight="1">
+    <row r="13" spans="1:6" ht="105">
       <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
@@ -4736,7 +4743,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19.5" customHeight="1">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="14" t="s">
         <v>69</v>
       </c>
@@ -4752,7 +4759,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19.5" customHeight="1">
+    <row r="15" spans="1:6" ht="75">
       <c r="A15" s="14" t="s">
         <v>19</v>
       </c>
@@ -4770,7 +4777,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19.5" customHeight="1">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="14" t="s">
         <v>20</v>
       </c>
@@ -4786,7 +4793,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19.5" customHeight="1">
+    <row r="17" spans="1:6" ht="195">
       <c r="A17" s="14" t="s">
         <v>21</v>
       </c>
@@ -4804,7 +4811,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="255">
       <c r="A18" s="14" t="s">
         <v>73</v>
       </c>
@@ -4822,7 +4829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+    <row r="19" spans="1:6" ht="45">
       <c r="A19" s="14" t="s">
         <v>74</v>
       </c>
@@ -4838,7 +4845,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="105">
       <c r="A20" s="14" t="s">
         <v>75</v>
       </c>
@@ -4854,7 +4861,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
@@ -4870,7 +4877,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19.5" customHeight="1">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19.5" customHeight="1">
+    <row r="23" spans="1:6" ht="105">
       <c r="A23" s="14" t="s">
         <v>76</v>
       </c>
@@ -4904,7 +4911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19.5" customHeight="1">
+    <row r="24" spans="1:6" ht="150">
       <c r="A24" s="14" t="s">
         <v>78</v>
       </c>
@@ -4922,7 +4929,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19.5" customHeight="1">
+    <row r="25" spans="1:6" ht="120">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -4940,7 +4947,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19.5" customHeight="1">
+    <row r="26" spans="1:6" ht="105">
       <c r="A26" s="14" t="s">
         <v>30</v>
       </c>
@@ -4958,7 +4965,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="19.5" customHeight="1">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="14" t="s">
         <v>83</v>
       </c>
@@ -4974,7 +4981,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1">
+    <row r="28" spans="1:6" ht="75">
       <c r="A28" s="14" t="s">
         <v>32</v>
       </c>
@@ -4992,7 +4999,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="19.5" customHeight="1">
+    <row r="29" spans="1:6" ht="30">
       <c r="A29" s="14" t="s">
         <v>33</v>
       </c>
@@ -5008,7 +5015,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="19.5" customHeight="1">
+    <row r="30" spans="1:6" ht="105">
       <c r="A30" s="14" t="s">
         <v>85</v>
       </c>
@@ -5026,7 +5033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="19.5" customHeight="1">
+    <row r="31" spans="1:6" ht="105">
       <c r="A31" s="14" t="s">
         <v>35</v>
       </c>
@@ -5044,7 +5051,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="19.5" customHeight="1">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="14" t="s">
         <v>88</v>
       </c>
@@ -5060,7 +5067,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="19.5" customHeight="1">
+    <row r="33" spans="1:6" ht="105">
       <c r="A33" s="14" t="s">
         <v>37</v>
       </c>
@@ -5078,7 +5085,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="19.5" customHeight="1">
+    <row r="34" spans="1:6" ht="90">
       <c r="A34" s="14" t="s">
         <v>38</v>
       </c>
@@ -5094,7 +5101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="19.5" customHeight="1">
+    <row r="35" spans="1:6" ht="90">
       <c r="A35" s="14" t="s">
         <v>39</v>
       </c>
@@ -5110,7 +5117,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="19.5" customHeight="1">
+    <row r="36" spans="1:6" ht="45">
       <c r="A36" s="14" t="s">
         <v>40</v>
       </c>
@@ -5126,7 +5133,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="19.5" customHeight="1">
+    <row r="37" spans="1:6" ht="30">
       <c r="A37" s="14" t="s">
         <v>41</v>
       </c>
@@ -5134,7 +5141,7 @@
       <c r="C37" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="16" t="s">
@@ -5144,7 +5151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="19.5" customHeight="1">
+    <row r="38" spans="1:6" ht="15">
       <c r="A38" s="14" t="s">
         <v>42</v>
       </c>
@@ -5160,7 +5167,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="19.5" customHeight="1">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="14" t="s">
         <v>43</v>
       </c>
@@ -5176,7 +5183,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="19.5" customHeight="1">
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="14" t="s">
         <v>92</v>
       </c>
@@ -5192,7 +5199,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="19.5" customHeight="1">
+    <row r="41" spans="1:6" ht="15">
       <c r="A41" s="14" t="s">
         <v>45</v>
       </c>
@@ -5208,7 +5215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="19.5" customHeight="1">
+    <row r="42" spans="1:6" ht="45">
       <c r="A42" s="14" t="s">
         <v>46</v>
       </c>
@@ -5439,11 +5446,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" style="25" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="107.5703125" customWidth="1"/>
     <col min="3" max="4" width="55" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
@@ -5466,7 +5476,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" customHeight="1">
+    <row r="2" spans="1:5" ht="262.5" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>117</v>
       </c>
@@ -5581,6 +5591,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Upgrade to AndroidApp-v5.0.1 v30
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC8F93-F7DB-4C66-9D0A-519AB39B7769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDE47FE-80B0-410E-9105-28580BEB94AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24300" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List with Pending or Done" sheetId="1" r:id="rId1"/>
@@ -1937,7 +1937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D388"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -3561,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD42"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3853,7 +3855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="240">
+    <row r="17" spans="1:6" ht="225">
       <c r="A17" s="14" t="s">
         <v>21</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="150">
+    <row r="25" spans="1:6" ht="135">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -4179,7 +4181,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60">
+    <row r="36" spans="1:6" ht="45">
       <c r="A36" s="14" t="s">
         <v>40</v>
       </c>
@@ -4507,7 +4509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A42" sqref="A2:XFD42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to KenpoFlashcardsWebServer-v6.0.0 v31
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDE47FE-80B0-410E-9105-28580BEB94AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0153C4-EC97-4F11-B44D-41B1B1C78AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="437">
   <si>
     <t>App</t>
   </si>
@@ -1399,6 +1399,18 @@
   </si>
   <si>
     <t>If you want parity on Android, add UI/logic in Android app; if server-only, document it under Web App Sync section.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App needs to have a way to change its url pushed from webserver or pushed from app admin to other users. I don’t want other users seeing my url in app.  </t>
+  </si>
+  <si>
+    <t>Webserver (ws) Need a button on all cards and decks to mark for custom deck, quick actions section each tab need to be highlighted when veiwing that tab.</t>
+  </si>
+  <si>
+    <t>WebserverPackage (wsp)  Windows still thinks the version installed is v1.0.0 that needs to be updated as it changes versions, sort all cards deck by status dropdown, nothing marked in "all" shows up in custom deck</t>
+  </si>
+  <si>
+    <t>Have custom deck also sync with other devices</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1950,7 @@
   <dimension ref="A1:D388"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2555,25 +2567,37 @@
     <row r="66" spans="1:4">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" ht="30">
+      <c r="A67" s="1" t="s">
+        <v>433</v>
+      </c>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" ht="30">
+      <c r="A69" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" ht="45">
+      <c r="A71" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4">
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4">
+      <c r="A73" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4">

</xml_diff>

<commit_message>
Upgrade to KenpoFlashcardsWebServer-v6.1.0 v32 and KenpoFlashcardsWebServer_Packaged-v1.3.0 v8
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0153C4-EC97-4F11-B44D-41B1B1C78AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D5A3B8-5BA6-4B10-A3F6-0052C7C0A1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1404,13 +1404,13 @@
     <t xml:space="preserve">App needs to have a way to change its url pushed from webserver or pushed from app admin to other users. I don’t want other users seeing my url in app.  </t>
   </si>
   <si>
-    <t>Webserver (ws) Need a button on all cards and decks to mark for custom deck, quick actions section each tab need to be highlighted when veiwing that tab.</t>
-  </si>
-  <si>
-    <t>WebserverPackage (wsp)  Windows still thinks the version installed is v1.0.0 that needs to be updated as it changes versions, sort all cards deck by status dropdown, nothing marked in "all" shows up in custom deck</t>
-  </si>
-  <si>
     <t>Have custom deck also sync with other devices</t>
+  </si>
+  <si>
+    <t>WebserverPackage (wsp)  Windows still thinks the version installed is v1.0.0 that needs to be updated as it changes versions,  An option in tray settings to auto start with system and open gui on start.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webserver (ws) Need a button near all cards and in all decks to mark for custom deck, no cards marked in "all" shows up in custom deck(keeps showing nothing there), make sure this work for all decks.  Quick actions section each tab need to be highlighted when veiwing that tab. Need a sync progress page in settings with Web App Sync like the App. Move login/logout to "User:*****",  change buttons in setting to be similur to apps buttons, and pages. Sort "all" cards deck by status dropdown, </t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1950,7 @@
   <dimension ref="A1:D388"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2576,9 +2576,9 @@
     <row r="68" spans="1:4">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" ht="30">
+    <row r="69" spans="1:4" ht="90">
       <c r="A69" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D69" s="2"/>
     </row>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D73" s="2"/>
     </row>

</xml_diff>

<commit_message>
Upgraded Package to 2.0.0 and Webserver to 6.2.0
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D5A3B8-5BA6-4B10-A3F6-0052C7C0A1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8093A4B2-BD7C-49C1-AF14-48F499D7F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,8 +31,40 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="442">
   <si>
     <t>App</t>
   </si>
@@ -1410,7 +1442,23 @@
     <t>WebserverPackage (wsp)  Windows still thinks the version installed is v1.0.0 that needs to be updated as it changes versions,  An option in tray settings to auto start with system and open gui on start.</t>
   </si>
   <si>
-    <t xml:space="preserve">Webserver (ws) Need a button near all cards and in all decks to mark for custom deck, no cards marked in "all" shows up in custom deck(keeps showing nothing there), make sure this work for all decks.  Quick actions section each tab need to be highlighted when veiwing that tab. Need a sync progress page in settings with Web App Sync like the App. Move login/logout to "User:*****",  change buttons in setting to be similur to apps buttons, and pages. Sort "all" cards deck by status dropdown, </t>
+    <t>in ws User guide page is basic and download user guide isnt working goes to a white page with "Internal Server Error
+The server encountered an internal error and was unable to complete your request. Either the server is overloaded or there is an error in the application."</t>
+  </si>
+  <si>
+    <t>in ws In admin "quick action" highlight is stuck on "Check Health", each tab need to be highlighted when veiwing that tab.  Can we make quick actions text look less cms promptish. Remove Card Groups section in Admin.  Replace with something cool.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort "all" cards deck by status dropdown, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webserver (ws) make reshuffle button same size as random toggle, I don’t like how everything below it moves down, only random toggle on custom page does not stay toggled. </t>
+  </si>
+  <si>
+    <t>in ws when clicked total users see users info, to give admin or to force password change, resetting to default 123456789 and require set new password.</t>
+  </si>
+  <si>
+    <t>The cards are there, not sure why it shows missing, the AI works on breakdowns, but the button does not work, and the Ai generated new card definitions has that error. When I manually add the fields, the add card button didn't do anything.</t>
   </si>
 </sst>
 </file>
@@ -1798,6 +1846,75 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1947,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D388"/>
+  <dimension ref="A1:D390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2576,10 +2693,7 @@
     <row r="68" spans="1:4">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" ht="90">
-      <c r="A69" s="1" t="s">
-        <v>436</v>
-      </c>
+    <row r="69" spans="1:4">
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4">
@@ -2604,69 +2718,93 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4">
+      <c r="A75" s="1" t="s">
+        <v>438</v>
+      </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" ht="30">
+      <c r="A76" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" ht="86.25" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" ht="45">
+      <c r="A78" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" ht="30">
+      <c r="A79" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4">
+    <row r="81" spans="1:4" ht="45">
+      <c r="A81" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B81" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C81" s="2" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4">
+    <row r="82" spans="1:4">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4">
+    <row r="83" spans="1:4">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4">
+    <row r="84" spans="1:4">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4">
+    <row r="85" spans="1:4">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4">
+    <row r="86" spans="1:4">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4">
+    <row r="87" spans="1:4">
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="4:4">
+    <row r="88" spans="1:4">
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="4:4">
+    <row r="89" spans="1:4">
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="4:4">
+    <row r="90" spans="1:4">
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="4:4">
+    <row r="91" spans="1:4">
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="4:4">
+    <row r="92" spans="1:4">
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="4:4">
+    <row r="93" spans="1:4">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4">
+    <row r="94" spans="1:4">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4">
+    <row r="95" spans="1:4">
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="4:4">
+    <row r="96" spans="1:4">
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="4:4">
@@ -3544,6 +3682,12 @@
     </row>
     <row r="388" spans="4:4">
       <c r="D388" s="2"/>
+    </row>
+    <row r="389" spans="4:4">
+      <c r="D389" s="2"/>
+    </row>
+    <row r="390" spans="4:4">
+      <c r="D390" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3565,7 +3709,7 @@
       <formula>C3="IN PROCESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:D388">
+  <conditionalFormatting sqref="C30:D390">
     <cfRule type="expression" dxfId="11" priority="1">
       <formula>C30="DONE"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated to KenpoFlashcardsWebServer-v7.0.3 v36
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B47A84A-39EA-4C11-B2A9-8FA4367E9511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BC1E26-FB21-41A4-A0E5-B2F88BC2E5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="442">
   <si>
     <t>App</t>
   </si>
@@ -2066,14 +2066,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="90" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="5" customWidth="1"/>
   </cols>
@@ -2729,23 +2729,33 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" ht="86.25" customHeight="1">
+    <row r="77" spans="1:4" ht="60.75" thickBot="1">
       <c r="A77" s="1" t="s">
         <v>436</v>
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" ht="45">
+    <row r="78" spans="1:4" ht="45.75" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" ht="30">
+      <c r="C78" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30.75" thickBot="1">
       <c r="A79" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="D79" s="2"/>
+      <c r="C79" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
       <c r="D80" s="2"/>

</xml_diff>

<commit_message>
Updating to 3.1.0.1 and repo org
</commit_message>
<xml_diff>
--- a/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
+++ b/App_Web_server_changes_to_be_merged_STATUS_BASELINE_Jan15_FEATURES_UPDATED (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidscri\Documents\GitHub\sidscri-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B86616-24A8-41D8-811F-CFEBACE0912E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51385CF5-37E9-4F1B-82A4-75D591E46665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="2160" windowWidth="13275" windowHeight="12690" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12945" yWindow="30" windowWidth="13275" windowHeight="12690" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List with Pending or Done" sheetId="1" r:id="rId1"/>
@@ -1500,10 +1500,10 @@
     <t xml:space="preserve">There isnt an option to either remove default then revert to the original or to swap default with the other kenpo study deck, since it has no default button and both say default. </t>
   </si>
   <si>
-    <t>In "custom set setting"; the number field for "Add Random" needs to be adjusted(shortened to be filled with 3 number, big of a field, with the same space on each end as it is now to the left of the 10).  I want the Custom Set Settings page to stay the same size for all tabs "Settings", "Manage Cards", "Saved Sets". Don’t like the current changing of windows sizes when going through empty tabs. Right now the "custom set setting" is bare. In "Custom"&gt;"Custom Set Setting"&gt;"Manage Cards"  need to be able to bulk remove or add Cards to or from selected Custom set, should show a list of cards in the deck to be removed, and should show a list of cards in the deck to added. "Custom"&gt;"Custom Set Setting"&gt;"Saved Sets" Need a save "Custom Deck" and be able to name the saved custom set, and to switch from between them, keeping all functions unique per custom deck.</t>
-  </si>
-  <si>
     <t>Is there a way to remove the built in status of kenpo?  I still want for now other users new and old to have this deck built in. In admin we I could have a danger section, where I can remove that Built-in lock at any time and I want specific users to have it built in or others without it.  Or setting for new users to have a blank deckless Study Flashcards app when they create thier account.  Would be great if only in admin I could have an auto generated (Something easy i.e "KenpoStudy409") invite code per deck for when used it unlockes decks for those users, deck shows up in "More"&gt;"Edit Decks"&gt;"Switch" as ("Unlocked" vs "Built-in"), or I can manually unlock. I want any changes made to the built-in/unlocked Study deck to be user specific, only changes made for that user, and a setting were I can block non admins from adding or removing from built-in/unlocked.</t>
+  </si>
+  <si>
+    <t>In "custom set setting"; the number field for "Add Random" needs to be adjusted(shortened to be filled with 3 number size of a field, with the same space on each end as it is now to the left of the 10) with it starting inline with the other.  I want the Custom Set Settings page to stay the same size for all tabs "Settings", "Manage Cards", "Saved Sets". Don’t like the current changing of windows sizes when going through empty tabs. Right now the "custom set setting" is bare. In "Custom"&gt;"Custom Set Setting"&gt;"Manage Cards"  need to be able to bulk remove or add Cards to or from selected Custom set, should show a list of cards in the deck to be removed, and should show a list of cards in the deck to added. "Custom"&gt;"Custom Set Setting"&gt;"Saved Sets" Need a save "Custom Deck" and be able to name the saved custom set, and to switch from between them, keeping all functions unique per custom deck.</t>
   </si>
 </sst>
 </file>
@@ -2198,14 +2198,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="90" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="5" customWidth="1"/>
   </cols>
@@ -2917,7 +2917,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="30">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="31" t="s">
         <v>443</v>
       </c>
       <c r="B82" s="2" t="e" vm="2">
@@ -2927,13 +2927,13 @@
     </row>
     <row r="83" spans="1:4" ht="150">
       <c r="A83" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="150">
       <c r="A84" s="31" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B84" s="2" t="e" vm="3">
         <v>#VALUE!</v>

</xml_diff>